<commit_message>
Update excel inicial 1
</commit_message>
<xml_diff>
--- a/Hamburgueria - PC/Excel/testingModel.xlsx
+++ b/Hamburgueria - PC/Excel/testingModel.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Hamburgueria\Hamburgueria - PC\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{62F027A0-8BE8-480F-AFAE-D7F2ECC6983F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{851B05B1-70F1-4C03-86D2-1EFB167D59E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{672D4E54-BFAB-4FBA-8964-D4F57280EE18}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{672D4E54-BFAB-4FBA-8964-D4F57280EE18}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
+    <sheet name="Planilha3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,8 +34,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -61,9 +71,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -380,7 +391,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B891944B-8995-40AB-906A-CCDE140ABF94}">
   <dimension ref="G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -393,4 +404,33 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0FFF54C-1711-46B1-8854-AB612172C86A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0511D62C-53FF-4DB1-92F4-3C7FBEC93E66}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Sale Day to Excel
</commit_message>
<xml_diff>
--- a/Hamburgueria - PC/Excel/testingModel.xlsx
+++ b/Hamburgueria - PC/Excel/testingModel.xlsx
@@ -5,17 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IGOR\Desktop\Hamburgueria\Hamburgueria - PC\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Hamburgueria\Hamburgueria - PC\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA70A7B4-082B-4CD4-8FB0-E489026126E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCEA5875-7E3F-4F3E-9235-73A106C62F50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{672D4E54-BFAB-4FBA-8964-D4F57280EE18}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{672D4E54-BFAB-4FBA-8964-D4F57280EE18}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
-    <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
-    <sheet name="Planilha3" sheetId="3" r:id="rId3"/>
+    <sheet name="Planilha3" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -103,9 +101,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -433,37 +430,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B891944B-8995-40AB-906A-CCDE140ABF94}">
-  <dimension ref="G2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="2" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G2" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0FFF54C-1711-46B1-8854-AB612172C86A}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0511D62C-53FF-4DB1-92F4-3C7FBEC93E66}">
   <dimension ref="A1:F1"/>
   <sheetViews>
@@ -471,31 +437,31 @@
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.77734375" style="7" customWidth="1"/>
-    <col min="2" max="2" width="30.77734375" style="2" customWidth="1"/>
-    <col min="3" max="5" width="30.77734375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="30.77734375" style="7" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" style="1" customWidth="1"/>
+    <col min="3" max="5" width="30.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="30.7109375" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>